<commit_message>
Worked on new branches list.
</commit_message>
<xml_diff>
--- a/spreadsheet/Hollard Branch List (Victor) 20170313 2055.xlsx
+++ b/spreadsheet/Hollard Branch List (Victor) 20170313 2055.xlsx
@@ -754,7 +754,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -776,6 +776,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -839,7 +845,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -969,6 +975,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="28">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -1434,11 +1446,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="217976192"/>
-        <c:axId val="217987328"/>
+        <c:axId val="219357568"/>
+        <c:axId val="219359104"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="217976192"/>
+        <c:axId val="219357568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1481,7 +1493,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="217987328"/>
+        <c:crossAx val="219359104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1489,7 +1501,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="217987328"/>
+        <c:axId val="219359104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1540,7 +1552,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="217976192"/>
+        <c:crossAx val="219357568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1910,7 +1922,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1924,7 +1936,7 @@
   <dimension ref="A1:H64"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1983,25 +1995,25 @@
       </c>
     </row>
     <row r="4" spans="1:8" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="50" t="s">
+      <c r="A4" s="73" t="s">
         <v>141</v>
       </c>
-      <c r="B4" s="50" t="s">
+      <c r="B4" s="73" t="s">
         <v>149</v>
       </c>
-      <c r="C4" s="50" t="s">
+      <c r="C4" s="73" t="s">
         <v>121</v>
       </c>
-      <c r="D4" s="50"/>
-      <c r="E4" s="50"/>
-      <c r="F4" s="50"/>
-      <c r="G4" s="51" t="s">
+      <c r="D4" s="73"/>
+      <c r="E4" s="73"/>
+      <c r="F4" s="73"/>
+      <c r="G4" s="74" t="s">
         <v>187</v>
       </c>
-      <c r="H4" s="52"/>
+      <c r="H4" s="75"/>
     </row>
     <row r="5" spans="1:8" s="45" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="53" t="s">
+      <c r="A5" s="76" t="s">
         <v>142</v>
       </c>
       <c r="B5" s="53" t="s">

</xml_diff>

<commit_message>
Final work on new branches list.
</commit_message>
<xml_diff>
--- a/spreadsheet/Hollard Branch List (Victor) 20170313 2055.xlsx
+++ b/spreadsheet/Hollard Branch List (Victor) 20170313 2055.xlsx
@@ -754,7 +754,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -764,12 +764,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -845,7 +839,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -931,22 +925,7 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -956,9 +935,30 @@
     <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="4" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -968,19 +968,7 @@
     <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="4" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="28">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -1446,11 +1434,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="219357568"/>
-        <c:axId val="219359104"/>
+        <c:axId val="126044800"/>
+        <c:axId val="126050688"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="219357568"/>
+        <c:axId val="126044800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1493,7 +1481,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="219359104"/>
+        <c:crossAx val="126050688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1501,7 +1489,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="219359104"/>
+        <c:axId val="126050688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1552,7 +1540,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="219357568"/>
+        <c:crossAx val="126044800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1935,8 +1923,10 @@
   </sheetPr>
   <dimension ref="A1:H64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1995,758 +1985,758 @@
       </c>
     </row>
     <row r="4" spans="1:8" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="73" t="s">
+      <c r="A4" s="60" t="s">
         <v>141</v>
       </c>
-      <c r="B4" s="73" t="s">
+      <c r="B4" s="60" t="s">
         <v>149</v>
       </c>
-      <c r="C4" s="73" t="s">
+      <c r="C4" s="60" t="s">
         <v>121</v>
       </c>
-      <c r="D4" s="73"/>
-      <c r="E4" s="73"/>
-      <c r="F4" s="73"/>
-      <c r="G4" s="74" t="s">
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="60"/>
+      <c r="G4" s="61" t="s">
         <v>187</v>
       </c>
-      <c r="H4" s="75"/>
+      <c r="H4" s="62"/>
     </row>
     <row r="5" spans="1:8" s="45" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="76" t="s">
+      <c r="A5" s="63" t="s">
         <v>142</v>
       </c>
-      <c r="B5" s="53" t="s">
+      <c r="B5" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="53" t="s">
+      <c r="C5" s="63" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="53"/>
-      <c r="E5" s="53"/>
-      <c r="F5" s="53"/>
-      <c r="G5" s="54" t="s">
+      <c r="D5" s="63"/>
+      <c r="E5" s="63"/>
+      <c r="F5" s="63"/>
+      <c r="G5" s="64" t="s">
         <v>188</v>
       </c>
-      <c r="H5" s="55"/>
+      <c r="H5" s="65"/>
     </row>
     <row r="6" spans="1:8" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="50" t="s">
+      <c r="A6" s="60" t="s">
         <v>142</v>
       </c>
-      <c r="B6" s="50" t="s">
+      <c r="B6" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="56" t="s">
+      <c r="C6" s="66" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="56"/>
-      <c r="E6" s="56"/>
-      <c r="F6" s="56"/>
-      <c r="G6" s="57" t="s">
+      <c r="D6" s="66"/>
+      <c r="E6" s="66"/>
+      <c r="F6" s="66"/>
+      <c r="G6" s="67" t="s">
         <v>189</v>
       </c>
-      <c r="H6" s="58" t="s">
+      <c r="H6" s="68" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="45" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A7" s="53" t="s">
+      <c r="A7" s="63" t="s">
         <v>143</v>
       </c>
-      <c r="B7" s="53" t="s">
+      <c r="B7" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="53" t="s">
+      <c r="C7" s="63" t="s">
         <v>152</v>
       </c>
-      <c r="D7" s="53"/>
-      <c r="E7" s="53"/>
-      <c r="F7" s="53"/>
-      <c r="G7" s="54" t="s">
+      <c r="D7" s="63"/>
+      <c r="E7" s="63"/>
+      <c r="F7" s="63"/>
+      <c r="G7" s="64" t="s">
         <v>190</v>
       </c>
-      <c r="H7" s="55"/>
+      <c r="H7" s="65"/>
     </row>
     <row r="8" spans="1:8" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A8" s="50" t="s">
+      <c r="A8" s="60" t="s">
         <v>144</v>
       </c>
-      <c r="B8" s="50" t="s">
+      <c r="B8" s="60" t="s">
         <v>150</v>
       </c>
-      <c r="C8" s="50" t="s">
+      <c r="C8" s="60" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="50"/>
-      <c r="E8" s="50"/>
-      <c r="F8" s="50"/>
-      <c r="G8" s="57" t="s">
+      <c r="D8" s="60"/>
+      <c r="E8" s="60"/>
+      <c r="F8" s="60"/>
+      <c r="G8" s="67" t="s">
         <v>191</v>
       </c>
-      <c r="H8" s="52"/>
+      <c r="H8" s="62"/>
     </row>
     <row r="9" spans="1:8" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="50" t="s">
+      <c r="A9" s="60" t="s">
         <v>145</v>
       </c>
-      <c r="B9" s="50" t="s">
+      <c r="B9" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="50" t="s">
+      <c r="C9" s="60" t="s">
         <v>46</v>
       </c>
-      <c r="D9" s="50"/>
-      <c r="E9" s="50"/>
-      <c r="F9" s="50"/>
-      <c r="G9" s="57" t="s">
+      <c r="D9" s="60"/>
+      <c r="E9" s="60"/>
+      <c r="F9" s="60"/>
+      <c r="G9" s="67" t="s">
         <v>192</v>
       </c>
-      <c r="H9" s="52"/>
+      <c r="H9" s="62"/>
     </row>
     <row r="10" spans="1:8" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="50" t="s">
+      <c r="A10" s="60" t="s">
         <v>142</v>
       </c>
-      <c r="B10" s="50" t="s">
+      <c r="B10" s="60" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="50" t="s">
+      <c r="C10" s="60" t="s">
         <v>42</v>
       </c>
-      <c r="D10" s="50"/>
-      <c r="E10" s="50"/>
-      <c r="F10" s="50"/>
-      <c r="G10" s="57" t="s">
+      <c r="D10" s="60"/>
+      <c r="E10" s="60"/>
+      <c r="F10" s="60"/>
+      <c r="G10" s="67" t="s">
         <v>193</v>
       </c>
-      <c r="H10" s="52"/>
+      <c r="H10" s="62"/>
     </row>
     <row r="11" spans="1:8" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A11" s="50" t="s">
+      <c r="A11" s="60" t="s">
         <v>146</v>
       </c>
-      <c r="B11" s="50" t="s">
+      <c r="B11" s="60" t="s">
         <v>49</v>
       </c>
-      <c r="C11" s="50" t="s">
+      <c r="C11" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="D11" s="50"/>
-      <c r="E11" s="50"/>
-      <c r="F11" s="50"/>
-      <c r="G11" s="51" t="s">
+      <c r="D11" s="60"/>
+      <c r="E11" s="60"/>
+      <c r="F11" s="60"/>
+      <c r="G11" s="61" t="s">
         <v>154</v>
       </c>
-      <c r="H11" s="52"/>
+      <c r="H11" s="62"/>
     </row>
     <row r="12" spans="1:8" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A12" s="50" t="s">
+      <c r="A12" s="60" t="s">
         <v>147</v>
       </c>
-      <c r="B12" s="50" t="s">
+      <c r="B12" s="60" t="s">
         <v>45</v>
       </c>
-      <c r="C12" s="50" t="s">
+      <c r="C12" s="60" t="s">
         <v>45</v>
       </c>
-      <c r="D12" s="50"/>
-      <c r="E12" s="50"/>
-      <c r="F12" s="50"/>
-      <c r="G12" s="57" t="s">
+      <c r="D12" s="60"/>
+      <c r="E12" s="60"/>
+      <c r="F12" s="60"/>
+      <c r="G12" s="67" t="s">
         <v>155</v>
       </c>
-      <c r="H12" s="52"/>
+      <c r="H12" s="62"/>
     </row>
     <row r="13" spans="1:8" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A13" s="50" t="s">
+      <c r="A13" s="60" t="s">
         <v>143</v>
       </c>
-      <c r="B13" s="50" t="s">
+      <c r="B13" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="50" t="s">
+      <c r="C13" s="60" t="s">
         <v>47</v>
       </c>
-      <c r="D13" s="50"/>
-      <c r="E13" s="50"/>
-      <c r="F13" s="50"/>
-      <c r="G13" s="50" t="s">
+      <c r="D13" s="60"/>
+      <c r="E13" s="60"/>
+      <c r="F13" s="60"/>
+      <c r="G13" s="60" t="s">
         <v>156</v>
       </c>
-      <c r="H13" s="52"/>
+      <c r="H13" s="62"/>
     </row>
     <row r="14" spans="1:8" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A14" s="50" t="s">
+      <c r="A14" s="60" t="s">
         <v>142</v>
       </c>
-      <c r="B14" s="50" t="s">
+      <c r="B14" s="60" t="s">
         <v>48</v>
       </c>
-      <c r="C14" s="50" t="s">
+      <c r="C14" s="60" t="s">
         <v>48</v>
       </c>
-      <c r="D14" s="50"/>
-      <c r="E14" s="50"/>
-      <c r="F14" s="50"/>
-      <c r="G14" s="59" t="s">
+      <c r="D14" s="60"/>
+      <c r="E14" s="60"/>
+      <c r="F14" s="60"/>
+      <c r="G14" s="69" t="s">
         <v>157</v>
       </c>
-      <c r="H14" s="52"/>
+      <c r="H14" s="62"/>
     </row>
     <row r="15" spans="1:8" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A15" s="50" t="s">
+      <c r="A15" s="60" t="s">
         <v>148</v>
       </c>
-      <c r="B15" s="50" t="s">
+      <c r="B15" s="60" t="s">
         <v>151</v>
       </c>
-      <c r="C15" s="50" t="s">
+      <c r="C15" s="60" t="s">
         <v>122</v>
       </c>
-      <c r="D15" s="50"/>
-      <c r="E15" s="50"/>
-      <c r="F15" s="50"/>
-      <c r="G15" s="57" t="s">
+      <c r="D15" s="60"/>
+      <c r="E15" s="60"/>
+      <c r="F15" s="60"/>
+      <c r="G15" s="67" t="s">
         <v>158</v>
       </c>
-      <c r="H15" s="52"/>
+      <c r="H15" s="62"/>
     </row>
     <row r="16" spans="1:8" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A16" s="50" t="s">
+      <c r="A16" s="60" t="s">
         <v>146</v>
       </c>
-      <c r="B16" s="50" t="s">
+      <c r="B16" s="60" t="s">
         <v>51</v>
       </c>
-      <c r="C16" s="50" t="s">
+      <c r="C16" s="60" t="s">
         <v>51</v>
       </c>
-      <c r="D16" s="50"/>
-      <c r="E16" s="50"/>
-      <c r="F16" s="50"/>
-      <c r="G16" s="57" t="s">
+      <c r="D16" s="60"/>
+      <c r="E16" s="60"/>
+      <c r="F16" s="60"/>
+      <c r="G16" s="67" t="s">
         <v>159</v>
       </c>
-      <c r="H16" s="52"/>
+      <c r="H16" s="62"/>
     </row>
     <row r="17" spans="1:8" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A17" s="50" t="s">
+      <c r="A17" s="60" t="s">
         <v>148</v>
       </c>
-      <c r="B17" s="50" t="s">
+      <c r="B17" s="60" t="s">
         <v>151</v>
       </c>
-      <c r="C17" s="50" t="s">
+      <c r="C17" s="60" t="s">
         <v>52</v>
       </c>
-      <c r="D17" s="50"/>
-      <c r="E17" s="50"/>
-      <c r="F17" s="50"/>
-      <c r="G17" s="57" t="s">
+      <c r="D17" s="60"/>
+      <c r="E17" s="60"/>
+      <c r="F17" s="60"/>
+      <c r="G17" s="67" t="s">
         <v>160</v>
       </c>
-      <c r="H17" s="52"/>
+      <c r="H17" s="62"/>
     </row>
     <row r="18" spans="1:8" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A18" s="50" t="s">
+      <c r="A18" s="60" t="s">
         <v>141</v>
       </c>
-      <c r="B18" s="60" t="s">
+      <c r="B18" s="70" t="s">
         <v>149</v>
       </c>
-      <c r="C18" s="50" t="s">
+      <c r="C18" s="60" t="s">
         <v>53</v>
       </c>
-      <c r="D18" s="50"/>
-      <c r="E18" s="50"/>
-      <c r="F18" s="50"/>
-      <c r="G18" s="50" t="s">
+      <c r="D18" s="60"/>
+      <c r="E18" s="60"/>
+      <c r="F18" s="60"/>
+      <c r="G18" s="60" t="s">
         <v>161</v>
       </c>
-      <c r="H18" s="52"/>
+      <c r="H18" s="62"/>
     </row>
     <row r="19" spans="1:8" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A19" s="50" t="s">
+      <c r="A19" s="60" t="s">
         <v>146</v>
       </c>
-      <c r="B19" s="50" t="s">
+      <c r="B19" s="60" t="s">
         <v>54</v>
       </c>
-      <c r="C19" s="50" t="s">
+      <c r="C19" s="60" t="s">
         <v>54</v>
       </c>
-      <c r="D19" s="50"/>
-      <c r="E19" s="50"/>
-      <c r="F19" s="50"/>
-      <c r="G19" s="57" t="s">
+      <c r="D19" s="60"/>
+      <c r="E19" s="60"/>
+      <c r="F19" s="60"/>
+      <c r="G19" s="67" t="s">
         <v>162</v>
       </c>
-      <c r="H19" s="52"/>
+      <c r="H19" s="62"/>
     </row>
     <row r="20" spans="1:8" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A20" s="50" t="s">
+      <c r="A20" s="60" t="s">
         <v>145</v>
       </c>
-      <c r="B20" s="50" t="s">
+      <c r="B20" s="60" t="s">
         <v>56</v>
       </c>
-      <c r="C20" s="50" t="s">
+      <c r="C20" s="60" t="s">
         <v>55</v>
       </c>
-      <c r="D20" s="50"/>
-      <c r="E20" s="50"/>
-      <c r="F20" s="50"/>
-      <c r="G20" s="57" t="s">
+      <c r="D20" s="60"/>
+      <c r="E20" s="60"/>
+      <c r="F20" s="60"/>
+      <c r="G20" s="67" t="s">
         <v>163</v>
       </c>
-      <c r="H20" s="52"/>
+      <c r="H20" s="62"/>
     </row>
     <row r="21" spans="1:8" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A21" s="50" t="s">
+      <c r="A21" s="60" t="s">
         <v>145</v>
       </c>
-      <c r="B21" s="50" t="s">
+      <c r="B21" s="60" t="s">
         <v>56</v>
       </c>
-      <c r="C21" s="50" t="s">
+      <c r="C21" s="60" t="s">
         <v>57</v>
       </c>
-      <c r="D21" s="50"/>
-      <c r="E21" s="50"/>
-      <c r="F21" s="50"/>
-      <c r="G21" s="61" t="s">
+      <c r="D21" s="60"/>
+      <c r="E21" s="60"/>
+      <c r="F21" s="60"/>
+      <c r="G21" s="71" t="s">
         <v>164</v>
       </c>
-      <c r="H21" s="52"/>
+      <c r="H21" s="62"/>
     </row>
     <row r="22" spans="1:8" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A22" s="50" t="s">
+      <c r="A22" s="60" t="s">
         <v>145</v>
       </c>
-      <c r="B22" s="50" t="s">
+      <c r="B22" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="50" t="s">
+      <c r="C22" s="60" t="s">
         <v>58</v>
       </c>
-      <c r="D22" s="50"/>
-      <c r="E22" s="50"/>
-      <c r="F22" s="50"/>
-      <c r="G22" s="59" t="s">
+      <c r="D22" s="60"/>
+      <c r="E22" s="60"/>
+      <c r="F22" s="60"/>
+      <c r="G22" s="69" t="s">
         <v>165</v>
       </c>
-      <c r="H22" s="52"/>
+      <c r="H22" s="62"/>
     </row>
     <row r="23" spans="1:8" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A23" s="50" t="s">
+      <c r="A23" s="60" t="s">
         <v>148</v>
       </c>
-      <c r="B23" s="50" t="s">
+      <c r="B23" s="60" t="s">
         <v>59</v>
       </c>
-      <c r="C23" s="62" t="s">
+      <c r="C23" s="72" t="s">
         <v>59</v>
       </c>
-      <c r="D23" s="62"/>
-      <c r="E23" s="62"/>
-      <c r="F23" s="62"/>
-      <c r="G23" s="50" t="s">
+      <c r="D23" s="72"/>
+      <c r="E23" s="72"/>
+      <c r="F23" s="72"/>
+      <c r="G23" s="60" t="s">
         <v>166</v>
       </c>
-      <c r="H23" s="50"/>
+      <c r="H23" s="60"/>
     </row>
     <row r="24" spans="1:8" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A24" s="50" t="s">
+      <c r="A24" s="60" t="s">
         <v>144</v>
       </c>
-      <c r="B24" s="50" t="s">
+      <c r="B24" s="60" t="s">
         <v>60</v>
       </c>
-      <c r="C24" s="50" t="s">
+      <c r="C24" s="60" t="s">
         <v>60</v>
       </c>
-      <c r="D24" s="50"/>
-      <c r="E24" s="50"/>
-      <c r="F24" s="50"/>
-      <c r="G24" s="50" t="s">
+      <c r="D24" s="60"/>
+      <c r="E24" s="60"/>
+      <c r="F24" s="60"/>
+      <c r="G24" s="60" t="s">
         <v>167</v>
       </c>
-      <c r="H24" s="50"/>
+      <c r="H24" s="60"/>
     </row>
     <row r="25" spans="1:8" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A25" s="63" t="s">
+      <c r="A25" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="B25" s="63" t="s">
+      <c r="B25" s="50" t="s">
         <v>87</v>
       </c>
-      <c r="C25" s="63" t="s">
+      <c r="C25" s="50" t="s">
         <v>61</v>
       </c>
-      <c r="D25" s="63"/>
-      <c r="E25" s="63"/>
-      <c r="F25" s="63"/>
-      <c r="G25" s="63" t="s">
+      <c r="D25" s="50"/>
+      <c r="E25" s="50"/>
+      <c r="F25" s="50"/>
+      <c r="G25" s="50" t="s">
         <v>168</v>
       </c>
-      <c r="H25" s="64"/>
+      <c r="H25" s="51"/>
     </row>
     <row r="26" spans="1:8" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A26" s="63" t="s">
+      <c r="A26" s="50" t="s">
         <v>142</v>
       </c>
-      <c r="B26" s="63" t="s">
+      <c r="B26" s="50" t="s">
         <v>62</v>
       </c>
-      <c r="C26" s="63" t="s">
+      <c r="C26" s="50" t="s">
         <v>62</v>
       </c>
-      <c r="D26" s="63"/>
-      <c r="E26" s="63"/>
-      <c r="F26" s="63"/>
-      <c r="G26" s="63" t="s">
+      <c r="D26" s="50"/>
+      <c r="E26" s="50"/>
+      <c r="F26" s="50"/>
+      <c r="G26" s="50" t="s">
         <v>169</v>
       </c>
-      <c r="H26" s="64"/>
+      <c r="H26" s="51"/>
     </row>
     <row r="27" spans="1:8" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A27" s="63" t="s">
+      <c r="A27" s="50" t="s">
         <v>141</v>
       </c>
-      <c r="B27" s="63" t="s">
+      <c r="B27" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="C27" s="63" t="s">
+      <c r="C27" s="50" t="s">
         <v>89</v>
       </c>
-      <c r="D27" s="63"/>
-      <c r="E27" s="63"/>
-      <c r="F27" s="63"/>
-      <c r="G27" s="63" t="s">
+      <c r="D27" s="50"/>
+      <c r="E27" s="50"/>
+      <c r="F27" s="50"/>
+      <c r="G27" s="50" t="s">
         <v>170</v>
       </c>
-      <c r="H27" s="64"/>
+      <c r="H27" s="51"/>
     </row>
     <row r="28" spans="1:8" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A28" s="63" t="s">
+      <c r="A28" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="B28" s="63" t="s">
+      <c r="B28" s="50" t="s">
         <v>88</v>
       </c>
-      <c r="C28" s="63" t="s">
+      <c r="C28" s="50" t="s">
         <v>88</v>
       </c>
-      <c r="D28" s="63"/>
-      <c r="E28" s="63"/>
-      <c r="F28" s="63"/>
-      <c r="G28" s="63" t="s">
+      <c r="D28" s="50"/>
+      <c r="E28" s="50"/>
+      <c r="F28" s="50"/>
+      <c r="G28" s="50" t="s">
         <v>171</v>
       </c>
-      <c r="H28" s="64"/>
+      <c r="H28" s="51"/>
     </row>
     <row r="29" spans="1:8" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A29" s="63" t="s">
+      <c r="A29" s="50" t="s">
         <v>148</v>
       </c>
-      <c r="B29" s="63" t="s">
+      <c r="B29" s="50" t="s">
         <v>63</v>
       </c>
-      <c r="C29" s="63" t="s">
+      <c r="C29" s="50" t="s">
         <v>63</v>
       </c>
-      <c r="D29" s="63"/>
-      <c r="E29" s="63"/>
-      <c r="F29" s="63"/>
-      <c r="G29" s="65" t="s">
+      <c r="D29" s="50"/>
+      <c r="E29" s="50"/>
+      <c r="F29" s="50"/>
+      <c r="G29" s="52" t="s">
         <v>172</v>
       </c>
-      <c r="H29" s="64"/>
+      <c r="H29" s="51"/>
     </row>
     <row r="30" spans="1:8" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A30" s="63" t="s">
+      <c r="A30" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="B30" s="63" t="s">
+      <c r="B30" s="50" t="s">
         <v>64</v>
       </c>
-      <c r="C30" s="63" t="s">
+      <c r="C30" s="50" t="s">
         <v>64</v>
       </c>
-      <c r="D30" s="63"/>
-      <c r="E30" s="63"/>
-      <c r="F30" s="63"/>
-      <c r="G30" s="63" t="s">
+      <c r="D30" s="50"/>
+      <c r="E30" s="50"/>
+      <c r="F30" s="50"/>
+      <c r="G30" s="50" t="s">
         <v>173</v>
       </c>
-      <c r="H30" s="64"/>
+      <c r="H30" s="51"/>
     </row>
     <row r="31" spans="1:8" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A31" s="63" t="s">
+      <c r="A31" s="50" t="s">
         <v>141</v>
       </c>
-      <c r="B31" s="66" t="s">
+      <c r="B31" s="53" t="s">
         <v>149</v>
       </c>
-      <c r="C31" s="63" t="s">
+      <c r="C31" s="50" t="s">
         <v>65</v>
       </c>
-      <c r="D31" s="63"/>
-      <c r="E31" s="63"/>
-      <c r="F31" s="63"/>
-      <c r="G31" s="67" t="s">
+      <c r="D31" s="50"/>
+      <c r="E31" s="50"/>
+      <c r="F31" s="50"/>
+      <c r="G31" s="54" t="s">
         <v>174</v>
       </c>
-      <c r="H31" s="64"/>
+      <c r="H31" s="51"/>
     </row>
     <row r="32" spans="1:8" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A32" s="63" t="s">
+      <c r="A32" s="50" t="s">
         <v>142</v>
       </c>
-      <c r="B32" s="63" t="s">
+      <c r="B32" s="50" t="s">
         <v>127</v>
       </c>
-      <c r="C32" s="63" t="s">
+      <c r="C32" s="50" t="s">
         <v>127</v>
       </c>
-      <c r="D32" s="63"/>
-      <c r="E32" s="63"/>
-      <c r="F32" s="63"/>
-      <c r="G32" s="63" t="s">
+      <c r="D32" s="50"/>
+      <c r="E32" s="50"/>
+      <c r="F32" s="50"/>
+      <c r="G32" s="50" t="s">
         <v>175</v>
       </c>
-      <c r="H32" s="63"/>
+      <c r="H32" s="50"/>
     </row>
     <row r="33" spans="1:8" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A33" s="63" t="s">
+      <c r="A33" s="50" t="s">
         <v>142</v>
       </c>
-      <c r="B33" s="63" t="s">
+      <c r="B33" s="50" t="s">
         <v>126</v>
       </c>
-      <c r="C33" s="63" t="s">
+      <c r="C33" s="50" t="s">
         <v>126</v>
       </c>
-      <c r="D33" s="63"/>
-      <c r="E33" s="63"/>
-      <c r="F33" s="63"/>
-      <c r="G33" s="63" t="s">
+      <c r="D33" s="50"/>
+      <c r="E33" s="50"/>
+      <c r="F33" s="50"/>
+      <c r="G33" s="50" t="s">
         <v>176</v>
       </c>
-      <c r="H33" s="63"/>
+      <c r="H33" s="50"/>
     </row>
     <row r="34" spans="1:8" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A34" s="63" t="s">
+      <c r="A34" s="50" t="s">
         <v>142</v>
       </c>
-      <c r="B34" s="63" t="s">
+      <c r="B34" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="C34" s="63" t="s">
+      <c r="C34" s="50" t="s">
         <v>125</v>
       </c>
-      <c r="D34" s="63"/>
-      <c r="E34" s="63"/>
-      <c r="F34" s="63"/>
-      <c r="G34" s="63" t="s">
+      <c r="D34" s="50"/>
+      <c r="E34" s="50"/>
+      <c r="F34" s="50"/>
+      <c r="G34" s="50" t="s">
         <v>177</v>
       </c>
-      <c r="H34" s="63"/>
+      <c r="H34" s="50"/>
     </row>
     <row r="35" spans="1:8" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A35" s="63" t="s">
+      <c r="A35" s="50" t="s">
         <v>142</v>
       </c>
-      <c r="B35" s="63" t="s">
+      <c r="B35" s="50" t="s">
         <v>92</v>
       </c>
-      <c r="C35" s="63" t="s">
+      <c r="C35" s="50" t="s">
         <v>92</v>
       </c>
-      <c r="D35" s="63"/>
-      <c r="E35" s="63"/>
-      <c r="F35" s="63"/>
-      <c r="G35" s="63" t="s">
+      <c r="D35" s="50"/>
+      <c r="E35" s="50"/>
+      <c r="F35" s="50"/>
+      <c r="G35" s="50" t="s">
         <v>178</v>
       </c>
-      <c r="H35" s="63"/>
+      <c r="H35" s="50"/>
     </row>
     <row r="36" spans="1:8" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A36" s="63" t="s">
+      <c r="A36" s="50" t="s">
         <v>141</v>
       </c>
-      <c r="B36" s="63" t="s">
+      <c r="B36" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="C36" s="63" t="s">
+      <c r="C36" s="50" t="s">
         <v>124</v>
       </c>
-      <c r="D36" s="63"/>
-      <c r="E36" s="63"/>
-      <c r="F36" s="63"/>
-      <c r="G36" s="63" t="s">
+      <c r="D36" s="50"/>
+      <c r="E36" s="50"/>
+      <c r="F36" s="50"/>
+      <c r="G36" s="50" t="s">
         <v>179</v>
       </c>
-      <c r="H36" s="63"/>
+      <c r="H36" s="50"/>
     </row>
     <row r="37" spans="1:8" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A37" s="63" t="s">
+      <c r="A37" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="B37" s="63" t="s">
+      <c r="B37" s="50" t="s">
         <v>123</v>
       </c>
-      <c r="C37" s="63" t="s">
+      <c r="C37" s="50" t="s">
         <v>123</v>
       </c>
-      <c r="D37" s="63"/>
-      <c r="E37" s="63"/>
-      <c r="F37" s="63"/>
-      <c r="G37" s="63" t="s">
+      <c r="D37" s="50"/>
+      <c r="E37" s="50"/>
+      <c r="F37" s="50"/>
+      <c r="G37" s="50" t="s">
         <v>180</v>
       </c>
-      <c r="H37" s="63"/>
+      <c r="H37" s="50"/>
     </row>
     <row r="38" spans="1:8" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A38" s="63" t="s">
+      <c r="A38" s="50" t="s">
         <v>142</v>
       </c>
-      <c r="B38" s="63" t="s">
+      <c r="B38" s="50" t="s">
         <v>67</v>
       </c>
-      <c r="C38" s="63" t="s">
+      <c r="C38" s="50" t="s">
         <v>153</v>
       </c>
-      <c r="D38" s="63"/>
-      <c r="E38" s="63"/>
-      <c r="F38" s="63"/>
-      <c r="G38" s="63"/>
-      <c r="H38" s="64"/>
+      <c r="D38" s="50"/>
+      <c r="E38" s="50"/>
+      <c r="F38" s="50"/>
+      <c r="G38" s="50"/>
+      <c r="H38" s="51"/>
     </row>
     <row r="39" spans="1:8" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A39" s="63" t="s">
+      <c r="A39" s="50" t="s">
         <v>142</v>
       </c>
-      <c r="B39" s="63" t="s">
+      <c r="B39" s="50" t="s">
         <v>69</v>
       </c>
-      <c r="C39" s="63" t="s">
+      <c r="C39" s="50" t="s">
         <v>68</v>
       </c>
-      <c r="D39" s="63"/>
-      <c r="E39" s="63"/>
-      <c r="F39" s="63"/>
-      <c r="G39" s="67" t="s">
+      <c r="D39" s="50"/>
+      <c r="E39" s="50"/>
+      <c r="F39" s="50"/>
+      <c r="G39" s="54" t="s">
         <v>181</v>
       </c>
-      <c r="H39" s="64"/>
+      <c r="H39" s="51"/>
     </row>
     <row r="40" spans="1:8" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A40" s="63" t="s">
+      <c r="A40" s="50" t="s">
         <v>142</v>
       </c>
-      <c r="B40" s="63" t="s">
+      <c r="B40" s="50" t="s">
         <v>92</v>
       </c>
-      <c r="C40" s="63" t="s">
+      <c r="C40" s="50" t="s">
         <v>91</v>
       </c>
-      <c r="D40" s="63"/>
-      <c r="E40" s="63"/>
-      <c r="F40" s="63"/>
-      <c r="G40" s="67" t="s">
+      <c r="D40" s="50"/>
+      <c r="E40" s="50"/>
+      <c r="F40" s="50"/>
+      <c r="G40" s="54" t="s">
         <v>92</v>
       </c>
-      <c r="H40" s="64"/>
+      <c r="H40" s="51"/>
     </row>
     <row r="41" spans="1:8" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A41" s="63" t="s">
+      <c r="A41" s="50" t="s">
         <v>142</v>
       </c>
-      <c r="B41" s="63" t="s">
+      <c r="B41" s="50" t="s">
         <v>93</v>
       </c>
-      <c r="C41" s="63" t="s">
+      <c r="C41" s="50" t="s">
         <v>93</v>
       </c>
-      <c r="D41" s="63"/>
-      <c r="E41" s="63"/>
-      <c r="F41" s="63"/>
-      <c r="G41" s="67" t="s">
+      <c r="D41" s="50"/>
+      <c r="E41" s="50"/>
+      <c r="F41" s="50"/>
+      <c r="G41" s="54" t="s">
         <v>182</v>
       </c>
-      <c r="H41" s="64"/>
+      <c r="H41" s="51"/>
     </row>
     <row r="42" spans="1:8" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A42" s="63" t="s">
+      <c r="A42" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="B42" s="63" t="s">
+      <c r="B42" s="50" t="s">
         <v>96</v>
       </c>
-      <c r="C42" s="63" t="s">
+      <c r="C42" s="50" t="s">
         <v>96</v>
       </c>
-      <c r="D42" s="63"/>
-      <c r="E42" s="63"/>
-      <c r="F42" s="63"/>
-      <c r="G42" s="68" t="s">
+      <c r="D42" s="50"/>
+      <c r="E42" s="50"/>
+      <c r="F42" s="50"/>
+      <c r="G42" s="55" t="s">
         <v>183</v>
       </c>
-      <c r="H42" s="64"/>
+      <c r="H42" s="51"/>
     </row>
     <row r="43" spans="1:8" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A43" s="63" t="s">
+      <c r="A43" s="50" t="s">
         <v>145</v>
       </c>
-      <c r="B43" s="63" t="s">
+      <c r="B43" s="50" t="s">
         <v>118</v>
       </c>
-      <c r="C43" s="63" t="s">
+      <c r="C43" s="50" t="s">
         <v>118</v>
       </c>
-      <c r="D43" s="63"/>
-      <c r="E43" s="63"/>
-      <c r="F43" s="63"/>
-      <c r="G43" s="67" t="s">
+      <c r="D43" s="50"/>
+      <c r="E43" s="50"/>
+      <c r="F43" s="50"/>
+      <c r="G43" s="54" t="s">
         <v>184</v>
       </c>
-      <c r="H43" s="64"/>
+      <c r="H43" s="51"/>
     </row>
     <row r="44" spans="1:8" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A44" s="63" t="s">
+      <c r="A44" s="50" t="s">
         <v>147</v>
       </c>
-      <c r="B44" s="63" t="s">
+      <c r="B44" s="50" t="s">
         <v>119</v>
       </c>
-      <c r="C44" s="63" t="s">
+      <c r="C44" s="50" t="s">
         <v>119</v>
       </c>
-      <c r="D44" s="63"/>
-      <c r="E44" s="63"/>
-      <c r="F44" s="63"/>
-      <c r="G44" s="69"/>
-      <c r="H44" s="64"/>
+      <c r="D44" s="50"/>
+      <c r="E44" s="50"/>
+      <c r="F44" s="50"/>
+      <c r="G44" s="56"/>
+      <c r="H44" s="51"/>
     </row>
     <row r="45" spans="1:8" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A45" s="63" t="s">
+      <c r="A45" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="B45" s="63" t="s">
+      <c r="B45" s="50" t="s">
         <v>66</v>
       </c>
-      <c r="C45" s="63" t="s">
+      <c r="C45" s="50" t="s">
         <v>66</v>
       </c>
-      <c r="D45" s="63"/>
-      <c r="E45" s="63"/>
-      <c r="F45" s="63"/>
-      <c r="G45" s="65" t="s">
+      <c r="D45" s="50"/>
+      <c r="E45" s="50"/>
+      <c r="F45" s="50"/>
+      <c r="G45" s="52" t="s">
         <v>185</v>
       </c>
-      <c r="H45" s="64"/>
+      <c r="H45" s="51"/>
     </row>
     <row r="46" spans="1:8" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="46" t="s">
@@ -2870,7 +2860,7 @@
       <c r="E54" s="46"/>
       <c r="F54" s="46"/>
       <c r="G54" s="48"/>
-      <c r="H54" s="70"/>
+      <c r="H54" s="57"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="46"/>
@@ -2881,8 +2871,8 @@
       <c r="D55" s="46"/>
       <c r="E55" s="46"/>
       <c r="F55" s="46"/>
-      <c r="G55" s="71"/>
-      <c r="H55" s="72"/>
+      <c r="G55" s="58"/>
+      <c r="H55" s="59"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="46"/>
@@ -2893,8 +2883,8 @@
       <c r="D56" s="46"/>
       <c r="E56" s="46"/>
       <c r="F56" s="46"/>
-      <c r="G56" s="71"/>
-      <c r="H56" s="72"/>
+      <c r="G56" s="58"/>
+      <c r="H56" s="59"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="46"/>
@@ -2905,8 +2895,8 @@
       <c r="D57" s="46"/>
       <c r="E57" s="46"/>
       <c r="F57" s="46"/>
-      <c r="G57" s="71"/>
-      <c r="H57" s="72"/>
+      <c r="G57" s="58"/>
+      <c r="H57" s="59"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="46"/>
@@ -2917,8 +2907,8 @@
       <c r="D58" s="46"/>
       <c r="E58" s="46"/>
       <c r="F58" s="46"/>
-      <c r="G58" s="71"/>
-      <c r="H58" s="72"/>
+      <c r="G58" s="58"/>
+      <c r="H58" s="59"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="46"/>
@@ -2929,8 +2919,8 @@
       <c r="D59" s="46"/>
       <c r="E59" s="46"/>
       <c r="F59" s="46"/>
-      <c r="G59" s="71"/>
-      <c r="H59" s="72"/>
+      <c r="G59" s="58"/>
+      <c r="H59" s="59"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="46"/>
@@ -2941,8 +2931,8 @@
       <c r="D60" s="46"/>
       <c r="E60" s="46"/>
       <c r="F60" s="46"/>
-      <c r="G60" s="71"/>
-      <c r="H60" s="72"/>
+      <c r="G60" s="58"/>
+      <c r="H60" s="59"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="46"/>
@@ -2953,8 +2943,8 @@
       <c r="D61" s="46"/>
       <c r="E61" s="46"/>
       <c r="F61" s="46"/>
-      <c r="G61" s="71"/>
-      <c r="H61" s="72"/>
+      <c r="G61" s="58"/>
+      <c r="H61" s="59"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="46"/>
@@ -2965,8 +2955,8 @@
       <c r="D62" s="46"/>
       <c r="E62" s="46"/>
       <c r="F62" s="46"/>
-      <c r="G62" s="71"/>
-      <c r="H62" s="72"/>
+      <c r="G62" s="58"/>
+      <c r="H62" s="59"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="46"/>
@@ -2977,8 +2967,8 @@
       <c r="D63" s="46"/>
       <c r="E63" s="46"/>
       <c r="F63" s="46"/>
-      <c r="G63" s="71"/>
-      <c r="H63" s="72"/>
+      <c r="G63" s="58"/>
+      <c r="H63" s="59"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="46"/>
@@ -2989,8 +2979,8 @@
       <c r="D64" s="46"/>
       <c r="E64" s="46"/>
       <c r="F64" s="46"/>
-      <c r="G64" s="71"/>
-      <c r="H64" s="72"/>
+      <c r="G64" s="58"/>
+      <c r="H64" s="59"/>
     </row>
   </sheetData>
   <autoFilter ref="C3:H64"/>

</xml_diff>